<commit_message>
Add milestone3 and update gantt
</commit_message>
<xml_diff>
--- a/docs/gantt-chart/Gantt Chart Excel.xlsx
+++ b/docs/gantt-chart/Gantt Chart Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailvalenciacc-my.sharepoint.com/personal/skissoonlall1_mail_valenciacollege_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C1558A6-E051-4FE8-9D99-A1854309D63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE818752-423A-4C80-98AF-FE0106AA6C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{EC9F1344-AAC9-46A4-98E0-BDD87C334DD5}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25335" windowHeight="14385" xr2:uid="{EC9F1344-AAC9-46A4-98E0-BDD87C334DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Valencia Medical Portal</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>Adjusted Length</t>
+  </si>
+  <si>
+    <t>Valencia Medical Portal</t>
   </si>
   <si>
     <t>Project Propsal</t>
@@ -78,20 +78,20 @@
     <t>Connecting Front-End Data to MySQL Tables</t>
   </si>
   <si>
+    <t>Final Deployment</t>
+  </si>
+  <si>
     <t>Implement Additions to UML Diagrams for the Back-End</t>
   </si>
   <si>
     <t>Testing and Quality Assurance</t>
-  </si>
-  <si>
-    <t>Final Deployment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,7 +487,7 @@
                   <c:v>45201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45201</c:v>
+                  <c:v>45209</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45219</c:v>
@@ -577,13 +577,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
@@ -1463,6 +1463,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1784,11 +1788,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDDBE5B-6F22-4C92-AA40-81CEC78E61A0}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" activeCellId="1" sqref="C9 C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
@@ -1797,34 +1801,34 @@
     <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="9.75" customHeight="1"/>
-    <row r="3" spans="1:5">
+    <row r="2" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1881,7 +1885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1889,18 +1893,18 @@
         <v>45187</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D7:D13" si="0">WORKDAY(B7,C7)</f>
-        <v>45201</v>
+        <f t="shared" ref="D7:D12" si="0">WORKDAY(B7,C7)</f>
+        <v>45215</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E13" si="1">D7-B7</f>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1908,26 +1912,26 @@
         <v>45201</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>45209</v>
+        <v>45215</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>45201</v>
+        <v>45209</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
@@ -1935,10 +1939,10 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1957,9 +1961,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>45239</v>
@@ -1976,9 +1980,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>45259</v>
@@ -1995,9 +1999,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>45261</v>
@@ -2014,13 +2018,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -2036,11 +2040,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BAC27A-6826-4383-B9EC-CEF5F10A4834}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2227,13 +2231,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F0E0D9C-3651-4ADF-AA13-21AD21C796D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F0E0D9C-3651-4ADF-AA13-21AD21C796D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e42e265a-e79a-4133-b0b0-90e1841b7878"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE3E2CD2-3766-4920-B07E-F0AC9E9DDF9E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE3E2CD2-3766-4920-B07E-F0AC9E9DDF9E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{136D5076-F8DC-4906-9117-201A51A1F245}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{136D5076-F8DC-4906-9117-201A51A1F245}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e42e265a-e79a-4133-b0b0-90e1841b7878"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>